<commit_message>
Add compute_para, derivatives, export_data.
</commit_message>
<xml_diff>
--- a/Fluid_Fractions_Produced_after_Breakthrough.xlsx
+++ b/Fluid_Fractions_Produced_after_Breakthrough.xlsx
@@ -1,36 +1,89 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ljin1\Dropbox\courses\2017s\MAP0000\MATLAB.Codes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libao Jin\Documents\Dropbox\courses\2017s\MAP0000\MAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Residues" sheetId="2" r:id="rId2"/>
+    <sheet name="Coefficients" sheetId="3" r:id="rId3"/>
+    <sheet name="S-r" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+  <si>
+    <t>TYPE1</t>
+  </si>
+  <si>
+    <t>TYPE2</t>
+  </si>
+  <si>
+    <t>TYPE3</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>k_rW / k_rO</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>tau</t>
+  </si>
+  <si>
+    <t>S_bar</t>
+  </si>
+  <si>
+    <t>S_outlet</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -61,9 +114,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,11 +403,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -1027,4 +1084,1256 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>9.4760827629270433E-2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>7.2862777427070605E-2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.11001294139251319</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3.3582643612450273E-2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.3258258813327371E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2.9127846080337728E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.7414160824228978E-2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>7.2921969964941068E-3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3.256918898422792E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.8274269030822764E-2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>7.3879403174940163E-3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4.4609742655385358E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-3.4756259682968462</v>
+      </c>
+      <c r="D2" s="2">
+        <v>12.844100093048754</v>
+      </c>
+      <c r="E2" s="2">
+        <v>-18.991671753042308</v>
+      </c>
+      <c r="F2" s="2">
+        <v>9.826772437020475</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-0.15266110763281537</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.662925140149851</v>
+      </c>
+      <c r="E3" s="2">
+        <v>-3.8268225472528918</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2.8329455539912956</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.14008658684504927</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.20983196475352878</v>
+      </c>
+      <c r="E4" s="2">
+        <v>-1.1011699146080103</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.2727561415881754</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.28443361222837876</v>
+      </c>
+      <c r="D5" s="2">
+        <v>-0.5279174651736861</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.42148316392744622</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.34177353119274645</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>-1.2258703517575882</v>
+      </c>
+      <c r="D6" s="2">
+        <v>6.5625663855616709</v>
+      </c>
+      <c r="E6" s="2">
+        <v>-12.080824936745115</v>
+      </c>
+      <c r="F6" s="2">
+        <v>7.0169645387175459</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-0.12117815083865262</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.4294056260500476</v>
+      </c>
+      <c r="E7" s="2">
+        <v>-3.7310626017747479</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2.7630168720156387</v>
+      </c>
+      <c r="G7" s="2">
+        <v>5.5100000000000003E-2</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.18959999999999999</v>
+      </c>
+      <c r="I7" s="2">
+        <v>-1.1889000000000001</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1.2861</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2">
+        <v>5.5105108241966315E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.18956950306962389</v>
+      </c>
+      <c r="E8" s="2">
+        <v>-1.1889409302263083</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.2861245498550777</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3</v>
+      </c>
+      <c r="H8" s="2">
+        <v>6</v>
+      </c>
+      <c r="I8" s="2">
+        <v>9</v>
+      </c>
+      <c r="J8" s="2">
+        <v>12</v>
+      </c>
+      <c r="K8" s="2">
+        <f>G7*G8</f>
+        <v>0.1653</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" ref="L8:N8" si="0">H7*H8</f>
+        <v>1.1375999999999999</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="0"/>
+        <v>-10.700100000000001</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="0"/>
+        <v>15.433199999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.13639580472667789</v>
+      </c>
+      <c r="D9" s="2">
+        <v>-0.47445764893223852</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.32791469376285987</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.3515560307006218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-0.33288088488893774</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2.1875048033799653</v>
+      </c>
+      <c r="E10" s="2">
+        <v>-4.6774733828110433</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3.3208057492855061</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.10477717418458354</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.24633598145058874</v>
+      </c>
+      <c r="E11" s="2">
+        <v>-1.0533911731846777</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1.2213556405507349</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.25875211665581094</v>
+      </c>
+      <c r="D12" s="2">
+        <v>-0.49052949192515422</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.56800735049483819</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.1802630973770967</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.40575869537831072</v>
+      </c>
+      <c r="D13" s="2">
+        <v>-1.2357859122103059</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2.2996442133601387</v>
+      </c>
+      <c r="F13" s="2">
+        <v>-0.95522279107239871</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.10282408982647158</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.38010956107519567</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.24115171818573691</v>
+      </c>
+      <c r="E2" s="2">
+        <v>-4.0382037609871566E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.13708744470908471</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.40903096291255531</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.31031600895871159</v>
+      </c>
+      <c r="E3" s="2">
+        <v>5.6750820259042462E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.17277985709424973</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.43101122830894867</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.35323093917579323</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.19080064884221642</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.20840421912215037</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.4460503572643757</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.37946134672393966</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.34365197963918603</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.24460700918679823</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.45819734603606666</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.39719635635635586</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.50811481897118704</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.28029942157196325</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.46541068390609053</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.40990086287327998</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.67612461709768279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.31657026199387539</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.4726240217761144</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.41998896431670135</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.85363174455752222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.3528751275944198</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.47609458999659748</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.42828897910511271</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.0401680460291605</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.39030282408982642</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.48099421571963252</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.43556283231090442</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.2438514420259374</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.42888737665872739</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.48531541340592044</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.44206705114375416</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.4677291837952389</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.46689350119088124</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.48905818305546112</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.44771237942839248</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.703389034529339</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.50489962572303504</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.49280095270500174</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.45274869463971301</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.9550367854123742</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.54147669275263688</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.49511466485199052</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.45711583514253423</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2.212962712177176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.57863218781898607</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.4971221503912896</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.46114101495281712</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2.4912398680216365</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.61490302824089826</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.49912963593058868</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.46472381879298313</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2.7790389515574252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.65059544062606323</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.4999802653963934</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.46795644110394585</v>
+      </c>
+      <c r="E17" s="2">
+        <v>3.0780576548285516</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.68659407961891794</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.50083089486219812</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.47095638023630404</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3.3957047184342173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.72490643075876149</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.50198775093569248</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.47389414220608117</v>
+      </c>
+      <c r="E19" s="2">
+        <v>3.7516417071464776</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.76063286832255872</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.50487989111942844</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.47642237988476255</v>
+      </c>
+      <c r="E20" s="2">
+        <v>4.1002724552724787</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.79693773392310308</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.5060367471929228</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.47880466184630222</v>
+      </c>
+      <c r="E21" s="2">
+        <v>4.4711623888225596</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.83409322898945215</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.50719360326641716</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.48106736586317439</v>
+      </c>
+      <c r="E22" s="2">
+        <v>4.8681546092565329</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.87097652262674374</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.50835045933991163</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.48315538708726674</v>
+      </c>
+      <c r="E23" s="2">
+        <v>5.2797167884922169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.90523987750935697</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.50950731541340599</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.48496732904103695</v>
+      </c>
+      <c r="E24" s="2">
+        <v>5.6776877579213094</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.9409663150731542</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.51008574345015312</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.48673754425088733</v>
+      </c>
+      <c r="E25" s="2">
+        <v>6.108732453400016</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.97665872745831916</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.51093637291595795</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.4883953418977065</v>
+      </c>
+      <c r="E26" s="2">
+        <v>6.55578737535863</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1.0138142225246682</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.51151480095270507</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.49001388170543703</v>
+      </c>
+      <c r="E27" s="2">
+        <v>7.0386291012123712</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1.0500850629465803</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.51294385845525692</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.4914975176841675</v>
+      </c>
+      <c r="E28" s="2">
+        <v>7.5271766111906979</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1.0843484178291936</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.51410071452875139</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.49281889336807749</v>
+      </c>
+      <c r="E29" s="2">
+        <v>8.0043101456876311</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1.1200408302143585</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.51495134399455611</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.49411924498242393</v>
+      </c>
+      <c r="E30" s="2">
+        <v>8.5175015673651782</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1.1583531813542021</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.51610820006805036</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.49543551635985</v>
+      </c>
+      <c r="E31" s="2">
+        <v>9.086723743852918</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1.1914937053419528</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.51641442667574011</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.49651283992102269</v>
+      </c>
+      <c r="E32" s="2">
+        <v>9.59445009298177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1.2231030962912555</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.51665260292616544</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.49749132060503237</v>
+      </c>
+      <c r="E33" s="2">
+        <v>10.091987933008244</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1.2614154474310988</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.5178094589996598</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.49861766811285024</v>
+      </c>
+      <c r="E34" s="2">
+        <v>10.712406793087105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1.2945559714188495</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.51784348417829196</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.49954296335745774</v>
+      </c>
+      <c r="E35" s="2">
+        <v>11.264439317168964</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1.3277305205852328</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.51818373596461387</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.50042686334545206</v>
+      </c>
+      <c r="E36" s="2">
+        <v>11.831318045404123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1.3597141884994892</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.51821776114324614</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.50124150747093899</v>
+      </c>
+      <c r="E37" s="2">
+        <v>12.391377779525795</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1.3939775433821022</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.51906839060905074</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.50207595794628312</v>
+      </c>
+      <c r="E38" s="2">
+        <v>13.006097502081905</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1.4271520925484855</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.51913644096631517</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.50284854955814362</v>
+      </c>
+      <c r="E39" s="2">
+        <v>13.615815157561913</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1.461687648860156</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.51998707043211989</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.503618229274441</v>
+      </c>
+      <c r="E40" s="2">
+        <v>14.265739443954464</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2">
+        <v>1.4933991153453552</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.52032732221844169</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.50429575954731454</v>
+      </c>
+      <c r="E41" s="2">
+        <v>14.87616841188234</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1.5277645457638649</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.52100782579108551</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.50500031693434355</v>
+      </c>
+      <c r="E42" s="2">
+        <v>15.552442828680686</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1.5623001020755356</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.52185845525689012</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.50567909911175868</v>
+      </c>
+      <c r="E43" s="2">
+        <v>16.247532323661702</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1.5965634569581486</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.52253895882953394</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.50632526382190024</v>
+      </c>
+      <c r="E44" s="2">
+        <v>16.952467832058243</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2">
+        <v>1.630520585233072</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.52281116025859142</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.50694041459898376</v>
+      </c>
+      <c r="E45" s="2">
+        <v>17.666164685733449</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2">
+        <v>1.6642735624362022</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.52315141204491333</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.5075283793355907</v>
+      </c>
+      <c r="E46" s="2">
+        <v>18.390431437634028</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2">
+        <v>1.6962572303504586</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.52318543722354549</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.50806509401768718</v>
+      </c>
+      <c r="E47" s="2">
+        <v>19.090405108569477</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2">
+        <v>1.7322558693433134</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.52376386526029273</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.50864670395526845</v>
+      </c>
+      <c r="E48" s="2">
+        <v>19.894163726386612</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="2">
+        <v>1.7667233752977196</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.5248186457978905</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.50918247371969139</v>
+      </c>
+      <c r="E49" s="2">
+        <v>20.679532975778066</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>